<commit_message>
Article updates - DAgger started
</commit_message>
<xml_diff>
--- a/Article/diagrams/DistributionalShift.xlsx
+++ b/Article/diagrams/DistributionalShift.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\IRL\IRL_for_PdM\Article\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD615446-87CE-4345-96DA-11E09F076F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145383CB-6DF6-401C-8F8C-31F196922C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="171" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,151 +219,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>3.1671241833119857E-5</c:v>
+                  <c:v>1.2238038602275437E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8389385158292053E-5</c:v>
+                  <c:v>2.4644383369460396E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2238038602275437E-4</c:v>
+                  <c:v>4.768176402929681E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4644383369460396E-4</c:v>
+                  <c:v>8.8636968238760153E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.768176402929681E-4</c:v>
+                  <c:v>1.5830903165959939E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8636968238760153E-4</c:v>
+                  <c:v>2.7165938467371225E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5830903165959939E-3</c:v>
+                  <c:v>4.4789060589685804E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7165938467371225E-3</c:v>
+                  <c:v>7.0949185692462842E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4789060589685804E-3</c:v>
+                  <c:v>1.0798193302637612E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0949185692462842E-3</c:v>
+                  <c:v>1.5790031660178828E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0798193302637612E-2</c:v>
+                  <c:v>2.2184166935891109E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5790031660178828E-2</c:v>
+                  <c:v>2.9945493127148972E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2184166935891109E-2</c:v>
+                  <c:v>3.8837210996642592E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9945493127148972E-2</c:v>
+                  <c:v>4.8394144903828672E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8837210996642592E-2</c:v>
+                  <c:v>5.7938310552296549E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.8394144903828672E-2</c:v>
+                  <c:v>6.6644920578359926E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.7938310552296549E-2</c:v>
+                  <c:v>7.3654028060664664E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.6644920578359926E-2</c:v>
+                  <c:v>7.8208538795091181E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.3654028060664664E-2</c:v>
+                  <c:v>7.9788456080286549E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7.8208538795091181E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.9788456080286549E-2</c:v>
+                  <c:v>7.3654028060664664E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.8208538795091181E-2</c:v>
+                  <c:v>6.6644920578359926E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.3654028060664664E-2</c:v>
+                  <c:v>5.7938310552296549E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.6644920578359926E-2</c:v>
+                  <c:v>4.8394144903828672E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.7938310552296549E-2</c:v>
+                  <c:v>3.8837210996642592E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.8394144903828672E-2</c:v>
+                  <c:v>2.9945493127148972E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.8837210996642592E-2</c:v>
+                  <c:v>2.2184166935891109E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.9945493127148972E-2</c:v>
+                  <c:v>1.5790031660178828E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2184166935891109E-2</c:v>
+                  <c:v>1.0798193302637612E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.5790031660178828E-2</c:v>
+                  <c:v>7.0949185692462842E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0798193302637612E-2</c:v>
+                  <c:v>4.4789060589685804E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.0949185692462842E-3</c:v>
+                  <c:v>2.7165938467371225E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.4789060589685804E-3</c:v>
+                  <c:v>1.5830903165959939E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.7165938467371225E-3</c:v>
+                  <c:v>8.8636968238760153E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.5830903165959939E-3</c:v>
+                  <c:v>4.768176402929681E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.8636968238760153E-4</c:v>
+                  <c:v>2.4644383369460396E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.768176402929681E-4</c:v>
+                  <c:v>1.2238038602275437E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.4644383369460396E-4</c:v>
+                  <c:v>5.8389385158292053E-5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.2238038602275437E-4</c:v>
+                  <c:v>2.6766045152977071E-5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.8389385158292053E-5</c:v>
+                  <c:v>1.1788613551307972E-5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.6766045152977071E-5</c:v>
+                  <c:v>4.9884942580107064E-6</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1788613551307972E-5</c:v>
+                  <c:v>2.0281704130973521E-6</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.9884942580107064E-6</c:v>
+                  <c:v>7.922598182064151E-7</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.0281704130973521E-6</c:v>
+                  <c:v>2.9734390294685955E-7</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.922598182064151E-7</c:v>
+                  <c:v>1.0722070689395228E-7</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.9734390294685955E-7</c:v>
+                  <c:v>3.7147236891105796E-8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.0722070689395228E-7</c:v>
+                  <c:v>1.2365241000331714E-8</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.7147236891105796E-8</c:v>
+                  <c:v>3.9546392812489344E-9</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.2365241000331714E-8</c:v>
+                  <c:v>1.2151765699646572E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -593,151 +593,151 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>3.7147236891105796E-8</c:v>
+                  <c:v>8.4993355868494329E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0722070689395228E-7</c:v>
+                  <c:v>3.4722760759568421E-10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9734390294685955E-7</c:v>
+                  <c:v>1.3501961888496192E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.922598182064151E-7</c:v>
+                  <c:v>4.9972705944367242E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0281704130973521E-6</c:v>
+                  <c:v>1.7604439974955947E-8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9884942580107064E-6</c:v>
+                  <c:v>5.902893130048695E-8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1788613551307972E-5</c:v>
+                  <c:v>1.8839136201309044E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6766045152977071E-5</c:v>
+                  <c:v>5.7228242699696244E-7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8389385158292053E-5</c:v>
+                  <c:v>1.654676860139998E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2238038602275437E-4</c:v>
+                  <c:v>4.5537515881941159E-6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4644383369460396E-4</c:v>
+                  <c:v>1.1928307789399006E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.768176402929681E-4</c:v>
+                  <c:v>2.9740050169974528E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.8636968238760153E-4</c:v>
+                  <c:v>7.0576142245008561E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5830903165959939E-3</c:v>
+                  <c:v>1.5941437969317927E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7165938467371225E-3</c:v>
+                  <c:v>3.4272866584246785E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.4789060589685804E-3</c:v>
+                  <c:v>7.0133695920400984E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.0949185692462842E-3</c:v>
+                  <c:v>1.3660178696914245E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0798193302637612E-2</c:v>
+                  <c:v>2.532441338621654E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5790031660178828E-2</c:v>
+                  <c:v>4.4686440943527616E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2184166935891109E-2</c:v>
+                  <c:v>7.5052557856156964E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9945493127148972E-2</c:v>
+                  <c:v>1.1997992558486235E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.8837210996642592E-2</c:v>
+                  <c:v>1.8255975213867966E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.8394144903828672E-2</c:v>
+                  <c:v>2.6439597872017006E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.7938310552296549E-2</c:v>
+                  <c:v>3.6446683261331922E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.6644920578359926E-2</c:v>
+                  <c:v>4.7820546889562457E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.3654028060664664E-2</c:v>
+                  <c:v>5.9720635898071993E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.8208538795091181E-2</c:v>
+                  <c:v>7.0988445671633829E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.9788456080286549E-2</c:v>
+                  <c:v>8.0316406640609669E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.8208538795091181E-2</c:v>
+                  <c:v>8.6491659815943631E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.3654028060664664E-2</c:v>
+                  <c:v>8.8653840089207264E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.6644920578359926E-2</c:v>
+                  <c:v>8.6491659815943631E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.7938310552296549E-2</c:v>
+                  <c:v>8.0316406640609669E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.8394144903828672E-2</c:v>
+                  <c:v>7.0988445671633829E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.8837210996642592E-2</c:v>
+                  <c:v>5.9720635898071993E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.9945493127148972E-2</c:v>
+                  <c:v>4.7820546889562457E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.2184166935891109E-2</c:v>
+                  <c:v>3.6446683261331922E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.5790031660178828E-2</c:v>
+                  <c:v>2.6439597872017006E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.0798193302637612E-2</c:v>
+                  <c:v>1.8255975213867966E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.0949185692462842E-3</c:v>
+                  <c:v>1.1997992558486235E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.4789060589685804E-3</c:v>
+                  <c:v>7.5052557856156964E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.7165938467371225E-3</c:v>
+                  <c:v>4.4686440943527616E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.5830903165959939E-3</c:v>
+                  <c:v>2.532441338621654E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>8.8636968238760153E-4</c:v>
+                  <c:v>1.3660178696914245E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.768176402929681E-4</c:v>
+                  <c:v>7.0133695920400984E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.4644383369460396E-4</c:v>
+                  <c:v>3.4272866584246785E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.2238038602275437E-4</c:v>
+                  <c:v>1.5941437969317927E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.8389385158292053E-5</c:v>
+                  <c:v>7.0576142245008561E-5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.6766045152977071E-5</c:v>
+                  <c:v>2.9740050169974528E-5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.1788613551307972E-5</c:v>
+                  <c:v>1.1928307789399006E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,6 +766,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -807,6 +821,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="5"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -869,7 +884,11 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1566,8 +1585,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8333423" y="1073634"/>
-          <a:ext cx="0" cy="2324100"/>
+          <a:off x="8258322" y="1121259"/>
+          <a:ext cx="0" cy="2447925"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1598,14 +1617,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>146437</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>556743</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>168759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>146437</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>556743</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>135628</xdr:rowOff>
     </xdr:to>
@@ -1622,8 +1641,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7847400" y="1073634"/>
-          <a:ext cx="0" cy="2319544"/>
+          <a:off x="7575935" y="1121259"/>
+          <a:ext cx="0" cy="2443369"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1655,13 +1674,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>219323</xdr:colOff>
+      <xdr:colOff>402497</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>168759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>219323</xdr:colOff>
+      <xdr:colOff>402497</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>135628</xdr:rowOff>
     </xdr:to>
@@ -1678,8 +1697,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8529886" y="1073634"/>
-          <a:ext cx="0" cy="2319544"/>
+          <a:off x="8637959" y="1121259"/>
+          <a:ext cx="0" cy="2443369"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2010,16 +2029,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63AEA97-2137-4A71-9B99-E6A6E650C327}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2033,47 +2052,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <f>_xlfn.NORM.DIST(A2,20,5,TRUE)</f>
-        <v>3.1671241833119857E-5</v>
+        <f>_xlfn.NORM.DIST(A2,18,5,FALSE)</f>
+        <v>1.2238038602275437E-4</v>
       </c>
       <c r="C2" s="2">
         <f>_xlfn.NORM.DIST($A2,25,3.5,FALSE)</f>
         <v>9.5038846503631718E-13</v>
       </c>
       <c r="D2" s="2">
-        <f>_xlfn.NORM.DIST($A2,27,5,FALSE)</f>
-        <v>3.7147236891105796E-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>_xlfn.NORM.DIST($A2,29,4.5,FALSE)</f>
+        <v>8.4993355868494329E-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B31" si="0">_xlfn.NORM.DIST(A3,20,5,FALSE)</f>
-        <v>5.8389385158292053E-5</v>
+        <f t="shared" ref="B3:B50" si="0">_xlfn.NORM.DIST(A3,18,5,FALSE)</f>
+        <v>2.4644383369460396E-4</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C50" si="1">_xlfn.NORM.DIST($A3,25,3.5,FALSE)</f>
         <v>7.0224736839299658E-12</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D50" si="2">_xlfn.NORM.DIST($A3,27,5,FALSE)</f>
-        <v>1.0722070689395228E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D3:D50" si="2">_xlfn.NORM.DIST($A3,29,4.5,FALSE)</f>
+        <v>3.4722760759568421E-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" si="0"/>
-        <v>1.2238038602275437E-4</v>
+        <v>4.768176402929681E-4</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="1"/>
@@ -2081,16 +2100,16 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="2"/>
-        <v>2.9734390294685955E-7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3501961888496192E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
-        <v>2.4644383369460396E-4</v>
+        <v>8.8636968238760153E-4</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
@@ -2098,16 +2117,16 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="2"/>
-        <v>7.922598182064151E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.9972705944367242E-9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
-        <v>4.768176402929681E-4</v>
+        <v>1.5830903165959939E-3</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
@@ -2115,16 +2134,16 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>2.0281704130973521E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.7604439974955947E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>8.8636968238760153E-4</v>
+        <v>2.7165938467371225E-3</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
@@ -2132,16 +2151,16 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>4.9884942580107064E-6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.902893130048695E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
-        <v>1.5830903165959939E-3</v>
+        <v>4.4789060589685804E-3</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -2149,16 +2168,16 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>1.1788613551307972E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.8839136201309044E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
-        <v>2.7165938467371225E-3</v>
+        <v>7.0949185692462842E-3</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -2166,16 +2185,16 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>2.6766045152977071E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.7228242699696244E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>4.4789060589685804E-3</v>
+        <v>1.0798193302637612E-2</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
@@ -2183,16 +2202,16 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>5.8389385158292053E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.654676860139998E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>7.0949185692462842E-3</v>
+        <v>1.5790031660178828E-2</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
@@ -2200,16 +2219,16 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>1.2238038602275437E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.5537515881941159E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>1.0798193302637612E-2</v>
+        <v>2.2184166935891109E-2</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="1"/>
@@ -2217,16 +2236,16 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="2"/>
-        <v>2.4644383369460396E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.1928307789399006E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>1.5790031660178828E-2</v>
+        <v>2.9945493127148972E-2</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="1"/>
@@ -2234,16 +2253,16 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>4.768176402929681E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.9740050169974528E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>2.2184166935891109E-2</v>
+        <v>3.8837210996642592E-2</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="1"/>
@@ -2251,16 +2270,16 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>8.8636968238760153E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0576142245008561E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>2.9945493127148972E-2</v>
+        <v>4.8394144903828672E-2</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
@@ -2268,16 +2287,16 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="2"/>
-        <v>1.5830903165959939E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5941437969317927E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>3.8837210996642592E-2</v>
+        <v>5.7938310552296549E-2</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
@@ -2285,16 +2304,16 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>2.7165938467371225E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.4272866584246785E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>4.8394144903828672E-2</v>
+        <v>6.6644920578359926E-2</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
@@ -2302,16 +2321,16 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>4.4789060589685804E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0133695920400984E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>5.7938310552296549E-2</v>
+        <v>7.3654028060664664E-2</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
@@ -2319,16 +2338,16 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="2"/>
-        <v>7.0949185692462842E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3660178696914245E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
-        <v>6.6644920578359926E-2</v>
+        <v>7.8208538795091181E-2</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
@@ -2336,16 +2355,16 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="2"/>
-        <v>1.0798193302637612E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.532441338621654E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
-        <v>7.3654028060664664E-2</v>
+        <v>7.9788456080286549E-2</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
@@ -2353,10 +2372,10 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>1.5790031660178828E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.4686440943527616E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2370,16 +2389,16 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="2"/>
-        <v>2.2184166935891109E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.5052557856156964E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>7.9788456080286549E-2</v>
+        <v>7.3654028060664664E-2</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="1"/>
@@ -2387,16 +2406,16 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" si="2"/>
-        <v>2.9945493127148972E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.1997992558486235E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
-        <v>7.8208538795091181E-2</v>
+        <v>6.6644920578359926E-2</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="1"/>
@@ -2404,16 +2423,16 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="2"/>
-        <v>3.8837210996642592E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.8255975213867966E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
-        <v>7.3654028060664664E-2</v>
+        <v>5.7938310552296549E-2</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="1"/>
@@ -2421,16 +2440,16 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="2"/>
-        <v>4.8394144903828672E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.6439597872017006E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
-        <v>6.6644920578359926E-2</v>
+        <v>4.8394144903828672E-2</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="1"/>
@@ -2438,16 +2457,16 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="2"/>
-        <v>5.7938310552296549E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.6446683261331922E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
-        <v>5.7938310552296549E-2</v>
+        <v>3.8837210996642592E-2</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="1"/>
@@ -2455,16 +2474,16 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="2"/>
-        <v>6.6644920578359926E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.7820546889562457E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
-        <v>4.8394144903828672E-2</v>
+        <v>2.9945493127148972E-2</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="1"/>
@@ -2472,16 +2491,16 @@
       </c>
       <c r="D27" s="2">
         <f t="shared" si="2"/>
-        <v>7.3654028060664664E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.9720635898071993E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
-        <v>3.8837210996642592E-2</v>
+        <v>2.2184166935891109E-2</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="1"/>
@@ -2489,16 +2508,16 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="2"/>
-        <v>7.8208538795091181E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0988445671633829E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
-        <v>2.9945493127148972E-2</v>
+        <v>1.5790031660178828E-2</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="1"/>
@@ -2506,16 +2525,16 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" si="2"/>
-        <v>7.9788456080286549E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.0316406640609669E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
-        <v>2.2184166935891109E-2</v>
+        <v>1.0798193302637612E-2</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="1"/>
@@ -2523,16 +2542,16 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="2"/>
-        <v>7.8208538795091181E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.6491659815943631E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="0"/>
-        <v>1.5790031660178828E-2</v>
+        <v>7.0949185692462842E-3</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="1"/>
@@ -2540,16 +2559,16 @@
       </c>
       <c r="D31" s="2">
         <f t="shared" si="2"/>
-        <v>7.3654028060664664E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.8653840089207264E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <f t="shared" ref="B32:B50" si="3">_xlfn.NORM.DIST(A32,20,5,FALSE)</f>
-        <v>1.0798193302637612E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4789060589685804E-3</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="1"/>
@@ -2557,16 +2576,16 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" si="2"/>
-        <v>6.6644920578359926E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.6491659815943631E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <f t="shared" si="3"/>
-        <v>7.0949185692462842E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.7165938467371225E-3</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="1"/>
@@ -2574,16 +2593,16 @@
       </c>
       <c r="D33" s="2">
         <f t="shared" si="2"/>
-        <v>5.7938310552296549E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.0316406640609669E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" s="2">
-        <f t="shared" si="3"/>
-        <v>4.4789060589685804E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.5830903165959939E-3</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="1"/>
@@ -2591,16 +2610,16 @@
       </c>
       <c r="D34" s="2">
         <f t="shared" si="2"/>
-        <v>4.8394144903828672E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0988445671633829E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" si="3"/>
-        <v>2.7165938467371225E-3</v>
+        <f t="shared" si="0"/>
+        <v>8.8636968238760153E-4</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="1"/>
@@ -2608,16 +2627,16 @@
       </c>
       <c r="D35" s="2">
         <f t="shared" si="2"/>
-        <v>3.8837210996642592E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.9720635898071993E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" si="3"/>
-        <v>1.5830903165959939E-3</v>
+        <f t="shared" si="0"/>
+        <v>4.768176402929681E-4</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="1"/>
@@ -2625,16 +2644,16 @@
       </c>
       <c r="D36" s="2">
         <f t="shared" si="2"/>
-        <v>2.9945493127148972E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.7820546889562457E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" si="3"/>
-        <v>8.8636968238760153E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.4644383369460396E-4</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="1"/>
@@ -2642,16 +2661,16 @@
       </c>
       <c r="D37" s="2">
         <f t="shared" si="2"/>
-        <v>2.2184166935891109E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.6446683261331922E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" si="3"/>
-        <v>4.768176402929681E-4</v>
+        <f t="shared" si="0"/>
+        <v>1.2238038602275437E-4</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="1"/>
@@ -2659,16 +2678,16 @@
       </c>
       <c r="D38" s="2">
         <f t="shared" si="2"/>
-        <v>1.5790031660178828E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.6439597872017006E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="2">
-        <f t="shared" si="3"/>
-        <v>2.4644383369460396E-4</v>
+        <f t="shared" si="0"/>
+        <v>5.8389385158292053E-5</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="1"/>
@@ -2676,16 +2695,16 @@
       </c>
       <c r="D39" s="2">
         <f t="shared" si="2"/>
-        <v>1.0798193302637612E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.8255975213867966E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" s="2">
-        <f t="shared" si="3"/>
-        <v>1.2238038602275437E-4</v>
+        <f t="shared" si="0"/>
+        <v>2.6766045152977071E-5</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="1"/>
@@ -2693,16 +2712,16 @@
       </c>
       <c r="D40" s="2">
         <f t="shared" si="2"/>
-        <v>7.0949185692462842E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.1997992558486235E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="2">
-        <f t="shared" si="3"/>
-        <v>5.8389385158292053E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.1788613551307972E-5</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="1"/>
@@ -2710,16 +2729,16 @@
       </c>
       <c r="D41" s="2">
         <f t="shared" si="2"/>
-        <v>4.4789060589685804E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.5052557856156964E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <f t="shared" si="3"/>
-        <v>2.6766045152977071E-5</v>
+        <f t="shared" si="0"/>
+        <v>4.9884942580107064E-6</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="1"/>
@@ -2727,16 +2746,16 @@
       </c>
       <c r="D42" s="2">
         <f t="shared" si="2"/>
-        <v>2.7165938467371225E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.4686440943527616E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="2">
-        <f t="shared" si="3"/>
-        <v>1.1788613551307972E-5</v>
+        <f t="shared" si="0"/>
+        <v>2.0281704130973521E-6</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="1"/>
@@ -2744,16 +2763,16 @@
       </c>
       <c r="D43" s="2">
         <f t="shared" si="2"/>
-        <v>1.5830903165959939E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.532441338621654E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" s="2">
-        <f t="shared" si="3"/>
-        <v>4.9884942580107064E-6</v>
+        <f t="shared" si="0"/>
+        <v>7.922598182064151E-7</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="1"/>
@@ -2761,16 +2780,16 @@
       </c>
       <c r="D44" s="2">
         <f t="shared" si="2"/>
-        <v>8.8636968238760153E-4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3660178696914245E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="2">
-        <f t="shared" si="3"/>
-        <v>2.0281704130973521E-6</v>
+        <f t="shared" si="0"/>
+        <v>2.9734390294685955E-7</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="1"/>
@@ -2778,16 +2797,16 @@
       </c>
       <c r="D45" s="2">
         <f t="shared" si="2"/>
-        <v>4.768176402929681E-4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0133695920400984E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" s="2">
-        <f t="shared" si="3"/>
-        <v>7.922598182064151E-7</v>
+        <f t="shared" si="0"/>
+        <v>1.0722070689395228E-7</v>
       </c>
       <c r="C46" s="2">
         <f t="shared" si="1"/>
@@ -2795,16 +2814,16 @@
       </c>
       <c r="D46" s="2">
         <f t="shared" si="2"/>
-        <v>2.4644383369460396E-4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.4272866584246785E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="2">
-        <f t="shared" si="3"/>
-        <v>2.9734390294685955E-7</v>
+        <f t="shared" si="0"/>
+        <v>3.7147236891105796E-8</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="1"/>
@@ -2812,16 +2831,16 @@
       </c>
       <c r="D47" s="2">
         <f t="shared" si="2"/>
-        <v>1.2238038602275437E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5941437969317927E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0722070689395228E-7</v>
+        <f t="shared" si="0"/>
+        <v>1.2365241000331714E-8</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="1"/>
@@ -2829,16 +2848,16 @@
       </c>
       <c r="D48" s="2">
         <f t="shared" si="2"/>
-        <v>5.8389385158292053E-5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0576142245008561E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" s="2">
-        <f t="shared" si="3"/>
-        <v>3.7147236891105796E-8</v>
+        <f t="shared" si="0"/>
+        <v>3.9546392812489344E-9</v>
       </c>
       <c r="C49" s="2">
         <f t="shared" si="1"/>
@@ -2846,16 +2865,16 @@
       </c>
       <c r="D49" s="2">
         <f t="shared" si="2"/>
-        <v>2.6766045152977071E-5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.9740050169974528E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" s="2">
-        <f t="shared" si="3"/>
-        <v>1.2365241000331714E-8</v>
+        <f t="shared" si="0"/>
+        <v>1.2151765699646572E-9</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" si="1"/>
@@ -2863,7 +2882,7 @@
       </c>
       <c r="D50" s="2">
         <f t="shared" si="2"/>
-        <v>1.1788613551307972E-5</v>
+        <v>1.1928307789399006E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Article: Added SLR table and funnel.
</commit_message>
<xml_diff>
--- a/Article/diagrams/DistributionalShift.xlsx
+++ b/Article/diagrams/DistributionalShift.xlsx
@@ -8,13 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\IRL\IRL_for_PdM\Article\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145383CB-6DF6-401C-8F8C-31F196922C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F9633-9310-4DC9-8D7B-55B888F5D0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="171" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="171" activeTab="1" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet2!$D$7:$D$9</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet2!$E$6</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet2!$E$7:$E$9</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet2!$E$32:$E$34</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet2!$F$31</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet2!$F$32:$F$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Original</t>
   </si>
@@ -38,12 +47,51 @@
   <si>
     <t>Learner</t>
   </si>
+  <si>
+    <t>Scopus</t>
+  </si>
+  <si>
+    <t>Web Of Science</t>
+  </si>
+  <si>
+    <t>Field of Inverse Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Applied to Robotics</t>
+  </si>
+  <si>
+    <t>Applied to Predictive Maintenance</t>
+  </si>
+  <si>
+    <t>Imitation Learning</t>
+  </si>
+  <si>
+    <t>Applied to PdM</t>
+  </si>
+  <si>
+    <t>IL applied to Robotics</t>
+  </si>
+  <si>
+    <t>IL applied to PdM</t>
+  </si>
+  <si>
+    <t>Field of Imitation Learning</t>
+  </si>
+  <si>
+    <t>("Inverse Reinforcement Learning" OR "Imitation Learning" OR "Apprenticeship Learning") AND ("predictive maintenance" OR "preventive maintenance" OR "prognostic")</t>
+  </si>
+  <si>
+    <t>IEEE Xplore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +104,20 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -86,6 +148,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,6 +1055,254 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Indexed Articles</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Indexed Articles</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{FCDF329C-42C2-4533-BD20-D709F0DABAE5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v2.1</cx:f>
+              <cx:v>Max </cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+            <cx:dataLabel idx="0">
+              <cx:txPr>
+                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr" rtl="0">
+                    <a:defRPr sz="2000" b="0">
+                      <a:solidFill>
+                        <a:srgbClr val="002060"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="002060"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                    </a:rPr>
+                    <a:t>4,966</a:t>
+                  </a:r>
+                </a:p>
+              </cx:txPr>
+              <cx:visibility seriesName="0" categoryName="0" value="1"/>
+            </cx:dataLabel>
+            <cx:dataLabel idx="1">
+              <cx:txPr>
+                <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="ctr" rtl="0">
+                    <a:defRPr sz="1600" b="0">
+                      <a:solidFill>
+                        <a:srgbClr val="002060"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="002060"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                    </a:rPr>
+                    <a:t>2,544</a:t>
+                  </a:r>
+                </a:p>
+              </cx:txPr>
+              <cx:visibility seriesName="0" categoryName="0" value="1"/>
+            </cx:dataLabel>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.0599999987"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v2.3</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v2.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Indexed Articles</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Indexed Articles</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="funnel" uniqueId="{D23C91B6-0C23-4B3E-A15E-737B1916764C}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v2.4</cx:f>
+              <cx:v>Scopus</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.0599999987"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -1005,6 +1340,18 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1517,6 +1864,1022 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1730,6 +3093,291 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>151088</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>149115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>6570</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>34815</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6EFD70A-A24D-4782-A451-41198EBF084A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6208988" y="697755"/>
+              <a:ext cx="4732282" cy="2628900"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>164225</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{351B29EE-C212-520A-156A-9011CC852BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8776139" y="2850931"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>358666</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>132036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>568872</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42042</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95A4C55-F20D-4CC3-A675-381990859606}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7637080" y="5282105"/>
+              <a:ext cx="4477406" cy="1560130"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>164225</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="288669" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{363ADDC5-A092-43AF-9C49-AFC0A86B9DD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8776139" y="2850931"/>
+          <a:ext cx="288669" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2029,16 +3677,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63AEA97-2137-4A71-9B99-E6A6E650C327}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2052,7 +3700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2069,7 +3717,7 @@
         <v>8.4993355868494329E-11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2086,7 +3734,7 @@
         <v>3.4722760759568421E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2103,7 +3751,7 @@
         <v>1.3501961888496192E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2120,7 +3768,7 @@
         <v>4.9972705944367242E-9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2137,7 +3785,7 @@
         <v>1.7604439974955947E-8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2154,7 +3802,7 @@
         <v>5.902893130048695E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2171,7 +3819,7 @@
         <v>1.8839136201309044E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2188,7 +3836,7 @@
         <v>5.7228242699696244E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2205,7 +3853,7 @@
         <v>1.654676860139998E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2222,7 +3870,7 @@
         <v>4.5537515881941159E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2239,7 +3887,7 @@
         <v>1.1928307789399006E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2256,7 +3904,7 @@
         <v>2.9740050169974528E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2273,7 +3921,7 @@
         <v>7.0576142245008561E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2290,7 +3938,7 @@
         <v>1.5941437969317927E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2307,7 +3955,7 @@
         <v>3.4272866584246785E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2324,7 +3972,7 @@
         <v>7.0133695920400984E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2341,7 +3989,7 @@
         <v>1.3660178696914245E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2358,7 +4006,7 @@
         <v>2.532441338621654E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2375,7 +4023,7 @@
         <v>4.4686440943527616E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2392,7 +4040,7 @@
         <v>7.5052557856156964E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2409,7 +4057,7 @@
         <v>1.1997992558486235E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2426,7 +4074,7 @@
         <v>1.8255975213867966E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2443,7 +4091,7 @@
         <v>2.6439597872017006E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2460,7 +4108,7 @@
         <v>3.6446683261331922E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2477,7 +4125,7 @@
         <v>4.7820546889562457E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2494,7 +4142,7 @@
         <v>5.9720635898071993E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2511,7 +4159,7 @@
         <v>7.0988445671633829E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2528,7 +4176,7 @@
         <v>8.0316406640609669E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2545,7 +4193,7 @@
         <v>8.6491659815943631E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2562,7 +4210,7 @@
         <v>8.8653840089207264E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2579,7 +4227,7 @@
         <v>8.6491659815943631E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2596,7 +4244,7 @@
         <v>8.0316406640609669E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2613,7 +4261,7 @@
         <v>7.0988445671633829E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2630,7 +4278,7 @@
         <v>5.9720635898071993E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2647,7 +4295,7 @@
         <v>4.7820546889562457E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2664,7 +4312,7 @@
         <v>3.6446683261331922E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2681,7 +4329,7 @@
         <v>2.6439597872017006E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2698,7 +4346,7 @@
         <v>1.8255975213867966E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2715,7 +4363,7 @@
         <v>1.1997992558486235E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2732,7 +4380,7 @@
         <v>7.5052557856156964E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2749,7 +4397,7 @@
         <v>4.4686440943527616E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2766,7 +4414,7 @@
         <v>2.532441338621654E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2783,7 +4431,7 @@
         <v>1.3660178696914245E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2800,7 +4448,7 @@
         <v>7.0133695920400984E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2817,7 +4465,7 @@
         <v>3.4272866584246785E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2834,7 +4482,7 @@
         <v>1.5941437969317927E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2851,7 +4499,7 @@
         <v>7.0576142245008561E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2868,7 +4516,7 @@
         <v>2.9740050169974528E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2884,6 +4532,213 @@
         <f t="shared" si="2"/>
         <v>1.1928307789399006E-5</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B067C0-7683-4CE7-96E4-3D398226135C}">
+  <dimension ref="B5:H46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="24.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="4"/>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7">
+        <f>MAX(F32:H32)</f>
+        <v>4966</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7">
+        <f>MAX(F33:H33)</f>
+        <v>2544</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <f>MAX(F34:H34)</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D29"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D30"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D31"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="7">
+        <v>4966</v>
+      </c>
+      <c r="G32" s="7">
+        <f>3516</f>
+        <v>3516</v>
+      </c>
+      <c r="H32" s="7">
+        <f>4679</f>
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="7">
+        <f>1632</f>
+        <v>1632</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1430</v>
+      </c>
+      <c r="H33" s="7">
+        <f>2544</f>
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="7">
+        <v>3</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D38"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D39"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D40"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D41"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D42"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D43"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D44"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D45"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D46"/>
+      <c r="E46" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Article: Added auto. vehicles to SLR table.
</commit_message>
<xml_diff>
--- a/Article/diagrams/DistributionalShift.xlsx
+++ b/Article/diagrams/DistributionalShift.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\IRL\IRL_for_PdM\Article\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F9633-9310-4DC9-8D7B-55B888F5D0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39566212-919E-4D21-B6E0-F976F3D69571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="171" activeTab="1" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet2!$D$7:$D$9</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet2!$E$6</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet2!$E$7:$E$9</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet2!$E$32:$E$34</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet2!$F$31</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet2!$F$32:$F$34</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet2!$E$32:$E$35</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet2!$F$31</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet2!$F$32:$F$35</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet2!$D$7:$D$10</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet2!$E$6</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet2!$E$7:$E$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Original</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t xml:space="preserve">Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">("Inverse Reinforcement Learning" OR "Imitation Learning" OR "Apprenticeship Learning") AND ("autonomous car" OR "autonomous vehicle" OR "autonomous driving" OR "self driving" OR "self-driving") </t>
+  </si>
+  <si>
+    <t>Applied to Autonomous Driving</t>
+  </si>
+  <si>
+    <t>IL applied to autonomous driving</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1069,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.0</cx:f>
+        <cx:f>_xlchart.v2.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v2.2</cx:f>
+        <cx:f>_xlchart.v2.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1101,7 +1110,7 @@
         <cx:series layoutId="funnel" uniqueId="{FCDF329C-42C2-4533-BD20-D709F0DABAE5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v2.1</cx:f>
+              <cx:f>_xlchart.v2.4</cx:f>
               <cx:v>Max </cx:v>
             </cx:txData>
           </cx:tx>
@@ -1220,89 +1229,6 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.3</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v2.5</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>Indexed Articles</cx:v>
-        </cx:txData>
-      </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>Indexed Articles</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
-    </cx:title>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="funnel" uniqueId="{D23C91B6-0C23-4B3E-A15E-737B1916764C}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v2.4</cx:f>
-              <cx:v>Scopus</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataLabels>
-            <cx:visibility seriesName="0" categoryName="0" value="1"/>
-          </cx:dataLabels>
-          <cx:dataId val="0"/>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0.0599999987"/>
-        <cx:tickLabels/>
-        <cx:txPr>
-          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:endParaRPr>
-          </a:p>
-        </cx:txPr>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -1346,12 +1272,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
-  <a:schemeClr val="accent5"/>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1869,514 +1789,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="419">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3142,7 +2554,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6208988" y="697755"/>
+              <a:off x="7329128" y="697755"/>
               <a:ext cx="4732282" cy="2628900"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3235,89 +2647,11 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>358666</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>132036</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>568872</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>42042</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" Requires="cx2">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Chart 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95A4C55-F20D-4CC3-A675-381990859606}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="7637080" y="5282105"/>
-              <a:ext cx="4477406" cy="1560130"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-IN" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>164225</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="288669" cy="342786"/>
@@ -4541,16 +3875,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B067C0-7683-4CE7-96E4-3D398226135C}">
-  <dimension ref="B5:H46"/>
+  <dimension ref="B5:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="24.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
     <col min="6" max="7" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4592,18 +3926,27 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>10</v>
+    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E9" s="7">
         <f>MAX(F34:H34)</f>
+        <v>754</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7">
+        <f>MAX(F35:H35)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="7"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D28" s="11" t="s">
@@ -4654,7 +3997,7 @@
         <v>4679</v>
       </c>
     </row>
-    <row r="33" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C33" s="8" t="s">
         <v>7</v>
       </c>
@@ -4674,71 +4017,92 @@
         <v>2544</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C34" s="8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D34"/>
       <c r="E34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="7">
+        <v>516</v>
+      </c>
+      <c r="G34" s="7">
+        <v>322</v>
+      </c>
+      <c r="H34" s="7">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F35" s="7">
         <v>3</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G35" s="7">
         <v>1</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H35" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D35"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D36"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D37"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D38"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D39"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D40"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D41"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="D42"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D43"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D44"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D45"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D46"/>
       <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D47"/>
+      <c r="E47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V.1.1 - Unfiltered and Zare comparison
</commit_message>
<xml_diff>
--- a/Article/diagrams/DistributionalShift.xlsx
+++ b/Article/diagrams/DistributionalShift.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\IRL\IRL_for_PdM\Article\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F599059-DD05-4B2B-8911-065A825E7446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413035F8-B3A0-4B9C-A99E-1E2345C778E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="460" activeTab="2" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="460" activeTab="1" xr2:uid="{FEE67D31-B0EB-4E24-95F6-1F8B5E92D37D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Zare Survey" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Zare Survey'!$A$1:$M$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Zare Survey'!$A$1:$L$71</definedName>
     <definedName name="_xlchart.v2.0" hidden="1">Sheet2!$D$7:$D$10</definedName>
     <definedName name="_xlchart.v2.1" hidden="1">Sheet2!$E$6</definedName>
     <definedName name="_xlchart.v2.2" hidden="1">Sheet2!$E$7:$E$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="240">
   <si>
     <t>Original</t>
   </si>
@@ -239,10 +243,6 @@
 Yes</t>
   </si>
   <si>
-    <t>Inverted Pendulum. Locomotion
-Insertion. Cable</t>
-  </si>
-  <si>
     <t>[20]</t>
   </si>
   <si>
@@ -345,18 +345,10 @@
     <t>Real</t>
   </si>
   <si>
-    <t>Predicting Driving Behavior,
-Route Recommendation</t>
-  </si>
-  <si>
     <t>[54]</t>
   </si>
   <si>
     <t>Maximum-margin IRL</t>
-  </si>
-  <si>
-    <t>Route Recommendation
-Route Planning</t>
   </si>
   <si>
     <t>[55]</t>
@@ -373,10 +365,6 @@
     <t>[56]</t>
   </si>
   <si>
-    <t>Footstep Prediction, Grasp Prediction,
-Navigation Task</t>
-  </si>
-  <si>
     <t>[57]</t>
   </si>
   <si>
@@ -390,10 +378,6 @@
   </si>
   <si>
     <t>[59]</t>
-  </si>
-  <si>
-    <t>System
-Robotic Manipulation</t>
   </si>
   <si>
     <t>[60]</t>
@@ -552,9 +536,6 @@
     <t>[81]</t>
   </si>
   <si>
-    <t>Physics-based Control. CoinRun Game</t>
-  </si>
-  <si>
     <t>[84]</t>
   </si>
   <si>
@@ -612,10 +593,6 @@
     <t>[103]</t>
   </si>
   <si>
-    <t>MiniGrid Environments, Robotic Manipulation
-Chess Game-endings</t>
-  </si>
-  <si>
     <t>[104]</t>
   </si>
   <si>
@@ -674,13 +651,139 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Inverted Pendulum. Locomotion</t>
+  </si>
+  <si>
+    <t>Route Recommendation, Route Planning</t>
+  </si>
+  <si>
+    <t>Path Planning and Route planning</t>
+  </si>
+  <si>
+    <t>Footstep Prediction, Grasp Prediction, Navigation Task</t>
+  </si>
+  <si>
+    <t>MiniGrid Environments, Robotic Manipulation, Chess Game-endings</t>
+  </si>
+  <si>
+    <t>Predicting Driving Behavior, Route Recommendation</t>
+  </si>
+  <si>
+    <t>Autonomous Driving; Robot</t>
+  </si>
+  <si>
+    <t>Games; Robot</t>
+  </si>
+  <si>
+    <t>Physics-based Control. Coin Run Game</t>
+  </si>
+  <si>
+    <t>Control tasks</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Application</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Articles</t>
+  </si>
+  <si>
+    <t>Robotics</t>
+  </si>
+  <si>
+    <t>Autonomous driving</t>
+  </si>
+  <si>
+    <t>IL Algorithm</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Behavioral Cloning</t>
+  </si>
+  <si>
+    <t>Application &amp; Articles &amp; %\\</t>
+  </si>
+  <si>
+    <t>Robotics &amp; 35 &amp; 46.67%\\</t>
+  </si>
+  <si>
+    <t>Games &amp; 15 &amp; 20.00%\\</t>
+  </si>
+  <si>
+    <t>Autonomous driving &amp; 13 &amp; 17.33%\\</t>
+  </si>
+  <si>
+    <t>Control tasks &amp; 5 &amp; 6.67%\\</t>
+  </si>
+  <si>
+    <t>Games &amp; 4 &amp; 5.33%\\</t>
+  </si>
+  <si>
+    <t>Path Planning and Route planning &amp; 3 &amp; 4.00%\\</t>
+  </si>
+  <si>
+    <t>IL Algorithm &amp; Articles &amp; %\\</t>
+  </si>
+  <si>
+    <t>Behavioral Cloning &amp; 17 &amp; 24.29%\\</t>
+  </si>
+  <si>
+    <t>Maximum Entropy IRL and Relative Entropy IRL &amp; 9 &amp; 12.86%\\</t>
+  </si>
+  <si>
+    <t>IRL others (IRL from Observations, Cross-embodiment IRL) &amp; 8 &amp; 11.43%\\</t>
+  </si>
+  <si>
+    <t>GAIL &amp; 7 &amp; 10.00%\\</t>
+  </si>
+  <si>
+    <t>Imitation from Observation &amp; 6 &amp; 8.57%\\</t>
+  </si>
+  <si>
+    <t>Bayesian IRL &amp; 5 &amp; 7.14%\\</t>
+  </si>
+  <si>
+    <t>Adversarial IRL &amp; 4 &amp; 5.71%\\</t>
+  </si>
+  <si>
+    <t>Maximum-margin IRL &amp; 4 &amp; 5.71%\\</t>
+  </si>
+  <si>
+    <t>Expert Support Estimation &amp; 3 &amp; 4.29%\\</t>
+  </si>
+  <si>
+    <t>Others &amp; 7 &amp; 10.00%\\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,8 +811,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +886,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -786,10 +914,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -873,9 +1002,53 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1828,28 +2001,28 @@
                   <c:v>BC</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Maximum Entropy IRL and Relative Entropy IRL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>IRL others (IRL from Observations, Cross-embodiment IRL)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GAIL</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Imitation from Observation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bayesian IRL</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Adversarial IRL</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>GAIL</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Maximum Entropy IRL and Relative Entropy IRL</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Bayesian IRL</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Maximum-margin IRL</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Expert Support Estimation</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>IRL others (IRL from Observations, Cross-embodiment IRL)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Imitation from Observation</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Others</c:v>
@@ -1867,28 +2040,28 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7</c:v>
@@ -1898,7 +2071,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E04B-4053-B7BD-7EAF31BA3D64}"/>
+              <c16:uniqueId val="{00000000-47FD-459D-A348-84FFFE754A3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1912,11 +2085,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1271593024"/>
-        <c:axId val="1271593504"/>
+        <c:axId val="817626624"/>
+        <c:axId val="817619904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1271593024"/>
+        <c:axId val="817626624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +2132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1271593504"/>
+        <c:crossAx val="817619904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1967,7 +2140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1271593504"/>
+        <c:axId val="817619904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,7 +2191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1271593024"/>
+        <c:crossAx val="817626624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4269,23 +4442,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1249680</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE5AED5-833A-0DAA-3E35-E6E98FEE4FDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5D5996-90DE-7165-76F3-5C407B4F0AB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4304,6 +4477,370 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rajesh Siraskar" refreshedDate="45552.721379861112" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="88" xr:uid="{C8003C0E-731A-4FEE-A8EB-B1B7A40AE4DE}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:A1048576" sheet="Sheet3"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Application" numFmtId="0">
+      <sharedItems containsBlank="1" count="8">
+        <s v="Robot"/>
+        <s v="Games"/>
+        <s v="Autonomous Driving"/>
+        <s v="Path Planning and Route planning"/>
+        <s v="Autonomous Driving; Robot"/>
+        <s v="Games; Robot"/>
+        <s v="Control tasks"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="88">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42D5120D-FB0C-4965-9573-843787402961}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I1:J10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="9">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Application" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5471,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B067C0-7683-4CE7-96E4-3D398226135C}">
   <dimension ref="B5:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5498,48 +6035,58 @@
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="7">
         <f>MAX(F32:H32)</f>
         <v>4966</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="7">
         <f>MAX(F33:H33)</f>
         <v>2544</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D9" s="3" t="s">
+      <c r="F8" s="43">
+        <f>E8/$E$7</f>
+        <v>0.51228352799033428</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="7">
         <f>MAX(F34:H34)</f>
         <v>754</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="43">
+        <f>E9/$E$7</f>
+        <v>0.15183246073298429</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="7">
         <f>MAX(F35:H35)</f>
         <v>3</v>
+      </c>
+      <c r="F10" s="43">
+        <f>E10/$E$7</f>
+        <v>6.0410793395086586E-4</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
@@ -5706,21 +6253,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5103FA80-FD93-4C2C-B44E-DBC3C8F3DE31}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="2" max="2" width="19.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" style="9" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="5"/>
-    <col min="7" max="7" width="38.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="5"/>
+    <col min="7" max="7" width="9.33203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5746,17 +6294,20 @@
       <c r="G1" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="H1" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="J1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L1">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -5775,14 +6326,17 @@
       <c r="F2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="32" t="s">
         <v>34</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -5801,14 +6355,17 @@
       <c r="F3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="17" t="s">
         <v>39</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -5827,14 +6384,17 @@
       <c r="F4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="17" t="s">
         <v>42</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -5853,14 +6413,17 @@
       <c r="F5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
         <v>47</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>48</v>
       </c>
@@ -5879,14 +6442,17 @@
       <c r="F6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="32" t="s">
         <v>50</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -5905,14 +6471,17 @@
       <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
         <v>47</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -5931,14 +6500,17 @@
       <c r="F8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
         <v>47</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -5957,14 +6529,17 @@
       <c r="F9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="32" t="s">
         <v>58</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>59</v>
       </c>
@@ -5984,15 +6559,18 @@
         <v>64</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>65</v>
+        <v>200</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>44</v>
@@ -6001,7 +6579,7 @@
         <v>36</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>32</v>
@@ -6009,16 +6587,19 @@
       <c r="F11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>29</v>
@@ -6027,7 +6608,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>32</v>
@@ -6035,16 +6616,19 @@
       <c r="F12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>202</v>
+      <c r="G12" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" t="s">
+        <v>206</v>
       </c>
       <c r="J12" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>29</v>
@@ -6053,7 +6637,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>32</v>
@@ -6061,16 +6645,19 @@
       <c r="F13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>44</v>
@@ -6079,7 +6666,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>32</v>
@@ -6087,16 +6674,19 @@
       <c r="F14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="34" t="s">
         <v>47</v>
       </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
       <c r="J14" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>29</v>
@@ -6105,24 +6695,27 @@
         <v>45</v>
       </c>
       <c r="D15" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>29</v>
@@ -6131,7 +6724,7 @@
         <v>45</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>32</v>
@@ -6139,16 +6732,19 @@
       <c r="F16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>83</v>
+      <c r="G16" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>29</v>
@@ -6157,7 +6753,7 @@
         <v>45</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>32</v>
@@ -6165,16 +6761,19 @@
       <c r="F17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>79</v>
+      <c r="G17" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J17" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>29</v>
@@ -6183,24 +6782,27 @@
         <v>45</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>79</v>
+      <c r="G18" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J18" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>29</v>
@@ -6209,24 +6811,27 @@
         <v>30</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" t="s">
+        <v>206</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>44</v>
@@ -6235,24 +6840,27 @@
         <v>30</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="32" t="s">
         <v>50</v>
       </c>
+      <c r="H20" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="J20" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>44</v>
@@ -6261,7 +6869,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>32</v>
@@ -6269,16 +6877,19 @@
       <c r="F21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>93</v>
+      <c r="G21" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>44</v>
@@ -6287,7 +6898,7 @@
         <v>45</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>32</v>
@@ -6295,16 +6906,19 @@
       <c r="F22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>29</v>
@@ -6313,7 +6927,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>32</v>
@@ -6321,25 +6935,28 @@
       <c r="F23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>32</v>
@@ -6347,25 +6964,28 @@
       <c r="F24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>99</v>
+      <c r="G24" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24" t="s">
+        <v>47</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>32</v>
@@ -6373,16 +6993,19 @@
       <c r="F25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>102</v>
+      <c r="G25" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="H25" t="s">
+        <v>202</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>44</v>
@@ -6391,7 +7014,7 @@
         <v>36</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>32</v>
@@ -6399,16 +7022,19 @@
       <c r="F26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>105</v>
+      <c r="G26" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" t="s">
+        <v>47</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>44</v>
@@ -6417,7 +7043,7 @@
         <v>36</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>32</v>
@@ -6425,16 +7051,19 @@
       <c r="F27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>107</v>
+      <c r="G27" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="H27" t="s">
+        <v>202</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>29</v>
@@ -6443,7 +7072,7 @@
         <v>45</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>32</v>
@@ -6451,16 +7080,19 @@
       <c r="F28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>109</v>
+      <c r="G28" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>29</v>
@@ -6469,7 +7101,7 @@
         <v>45</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>32</v>
@@ -6478,24 +7110,27 @@
         <v>38</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>32</v>
@@ -6503,16 +7138,19 @@
       <c r="F30" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>113</v>
+      <c r="G30" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>29</v>
@@ -6521,7 +7159,7 @@
         <v>45</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>32</v>
@@ -6529,16 +7167,19 @@
       <c r="F31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>116</v>
+      <c r="G31" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>29</v>
@@ -6547,7 +7188,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>32</v>
@@ -6555,16 +7196,19 @@
       <c r="F32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>116</v>
+      <c r="G32" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>29</v>
@@ -6573,7 +7217,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>32</v>
@@ -6582,15 +7226,18 @@
         <v>38</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>44</v>
@@ -6599,7 +7246,7 @@
         <v>45</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>32</v>
@@ -6607,16 +7254,19 @@
       <c r="F34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="32" t="s">
         <v>50</v>
       </c>
+      <c r="H34" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="J34" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>29</v>
@@ -6625,7 +7275,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>32</v>
@@ -6633,16 +7283,19 @@
       <c r="F35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>124</v>
+      <c r="G35" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>29</v>
@@ -6651,7 +7304,7 @@
         <v>45</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>32</v>
@@ -6660,15 +7313,18 @@
         <v>38</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>29</v>
@@ -6677,18 +7333,21 @@
         <v>45</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="G37" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="H37" t="s">
+        <v>47</v>
       </c>
       <c r="J37" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>29</v>
@@ -6697,18 +7356,21 @@
         <v>54</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>132</v>
+        <v>118</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>44</v>
@@ -6717,18 +7379,21 @@
         <v>45</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>29</v>
@@ -6737,18 +7402,21 @@
         <v>54</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J40" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>29</v>
@@ -6757,18 +7425,21 @@
         <v>45</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>29</v>
@@ -6777,18 +7448,21 @@
         <v>45</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
+      </c>
+      <c r="G42" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>29</v>
@@ -6797,18 +7471,21 @@
         <v>45</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>29</v>
@@ -6817,18 +7494,21 @@
         <v>45</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>29</v>
@@ -6837,18 +7517,21 @@
         <v>45</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>29</v>
@@ -6857,18 +7540,21 @@
         <v>45</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>79</v>
+        <v>131</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>29</v>
@@ -6877,18 +7563,21 @@
         <v>45</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>79</v>
+        <v>131</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J47" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>29</v>
@@ -6897,18 +7586,21 @@
         <v>30</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>152</v>
+        <v>140</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>29</v>
@@ -6917,10 +7609,13 @@
         <v>30</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>154</v>
+        <v>192</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="H49" t="s">
+        <v>47</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>32</v>
@@ -6928,7 +7623,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>44</v>
@@ -6937,18 +7632,21 @@
         <v>54</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G50" s="32" t="s">
         <v>50</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J50" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>44</v>
@@ -6957,10 +7655,13 @@
         <v>54</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>32</v>
@@ -6968,7 +7669,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>29</v>
@@ -6977,10 +7678,13 @@
         <v>45</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>32</v>
@@ -6988,7 +7692,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>29</v>
@@ -6997,10 +7701,13 @@
         <v>45</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>32</v>
@@ -7008,7 +7715,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>29</v>
@@ -7017,10 +7724,13 @@
         <v>36</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>164</v>
+        <v>151</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>32</v>
@@ -7028,7 +7738,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>29</v>
@@ -7037,10 +7747,13 @@
         <v>36</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>162</v>
+        <v>190</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>32</v>
@@ -7048,7 +7761,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>29</v>
@@ -7057,10 +7770,13 @@
         <v>45</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>79</v>
+        <v>151</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J56" s="5" t="s">
         <v>32</v>
@@ -7068,7 +7784,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>29</v>
@@ -7077,10 +7793,13 @@
         <v>45</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>79</v>
+        <v>162</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>32</v>
@@ -7088,7 +7807,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>29</v>
@@ -7097,18 +7816,21 @@
         <v>45</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>143</v>
+        <v>164</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>29</v>
@@ -7117,10 +7839,13 @@
         <v>54</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>132</v>
+        <v>151</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="J59" s="5" t="s">
         <v>32</v>
@@ -7128,7 +7853,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>29</v>
@@ -7137,10 +7862,13 @@
         <v>36</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>173</v>
+        <v>162</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>32</v>
@@ -7148,7 +7876,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>44</v>
@@ -7157,18 +7885,21 @@
         <v>54</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="G61" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G61" s="34" t="s">
         <v>47</v>
       </c>
+      <c r="H61" t="s">
+        <v>47</v>
+      </c>
       <c r="J61" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>29</v>
@@ -7177,18 +7908,21 @@
         <v>45</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>79</v>
+        <v>191</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J62" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>29</v>
@@ -7197,18 +7931,21 @@
         <v>45</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>79</v>
+        <v>172</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>29</v>
@@ -7217,18 +7954,21 @@
         <v>36</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="G64" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>29</v>
@@ -7237,18 +7977,21 @@
         <v>45</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>79</v>
+        <v>176</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>29</v>
@@ -7257,18 +8000,21 @@
         <v>45</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>184</v>
+        <v>85</v>
+      </c>
+      <c r="G66" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>29</v>
@@ -7277,18 +8023,21 @@
         <v>45</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>79</v>
+        <v>179</v>
+      </c>
+      <c r="G67" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>29</v>
@@ -7297,18 +8046,18 @@
         <v>45</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>44</v>
@@ -7317,18 +8066,21 @@
         <v>54</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="G69" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G69" s="32" t="s">
         <v>50</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>29</v>
@@ -7337,18 +8089,21 @@
         <v>45</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>143</v>
+        <v>188</v>
+      </c>
+      <c r="G70" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>29</v>
@@ -7357,119 +8112,1071 @@
         <v>45</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="G71" s="9" t="s">
-        <v>193</v>
+        <v>85</v>
+      </c>
+      <c r="G71" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F74" s="5">
+        <f>SUM(F75:F80)</f>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C76" s="14">
-        <f>SUM(C77:C90)</f>
-        <v>70</v>
+        <v>189</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="E76" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F76" s="5">
+        <v>35</v>
+      </c>
+      <c r="G76" s="29">
+        <f>F76/$F$74</f>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B77" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="5">
         <v>17</v>
       </c>
+      <c r="D77" s="29">
+        <f>C77/$C$88</f>
+        <v>0.24285714285714285</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" s="5">
+        <v>13</v>
+      </c>
+      <c r="G77" s="29">
+        <f>F77/$F$74</f>
+        <v>0.16883116883116883</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B78" s="23" t="s">
-        <v>145</v>
+      <c r="B78" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="C78" s="5">
+        <v>9</v>
+      </c>
+      <c r="D78" s="29">
+        <f t="shared" ref="D78:D86" si="0">C78/$C$88</f>
+        <v>0.12857142857142856</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F78" s="5">
+        <v>14</v>
+      </c>
+      <c r="G78" s="29">
+        <f>F78/$F$74</f>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="5">
+        <v>8</v>
+      </c>
+      <c r="D79" s="29">
+        <f t="shared" si="0"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F79" s="5">
+        <v>5</v>
+      </c>
+      <c r="G79" s="29">
+        <f>F79/$F$74</f>
+        <v>6.4935064935064929E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="5">
+        <v>7</v>
+      </c>
+      <c r="D80" s="29">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E80" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="F80" s="5">
+        <v>10</v>
+      </c>
+      <c r="G80" s="29">
+        <f>F80/$F$74</f>
+        <v>0.12987012987012986</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B81" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C81" s="5">
+        <v>6</v>
+      </c>
+      <c r="D81" s="29">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="G81" s="29"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B82" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="5">
+        <v>5</v>
+      </c>
+      <c r="D82" s="29">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="G82" s="29"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B79" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="C79" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B80" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C80" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C81" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C82" s="5">
+      <c r="D83" s="29">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G83" s="29"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B84" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="5">
+      <c r="D84" s="29">
+        <f t="shared" si="0"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F84" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B85" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C85" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="C84" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="29">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142858E-2</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F85" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" s="27" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C86" s="5">
         <v>7</v>
       </c>
+      <c r="D86" s="29">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F86" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E87" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F87" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C88" s="5">
+        <f>SUM(C77:C86)</f>
+        <v>70</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F88" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E89" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F89" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E90" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F90" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E92" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F92" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E95" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G95" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="H95" t="str">
+        <f>_xlfn.CONCAT(E95," &amp; ",TEXT(F95,0)," &amp; ",TEXT(G95,".00%"), "\\")</f>
+        <v>Application &amp; Articles &amp; %\\</v>
+      </c>
+      <c r="I95" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E96" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F96" s="40">
+        <f>29+4+2</f>
+        <v>35</v>
+      </c>
+      <c r="G96" s="39">
+        <f>F96/$F$103</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="H96" t="str">
+        <f t="shared" ref="H96:H101" si="1">_xlfn.CONCAT(E96," &amp; ",TEXT(F96,0)," &amp; ",TEXT(G96,".00%"), "\\")</f>
+        <v>Robotics &amp; 35 &amp; 46.67%\\</v>
+      </c>
+      <c r="I96" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="97" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E97" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F97" s="40">
+        <v>15</v>
+      </c>
+      <c r="G97" s="39">
+        <f t="shared" ref="G97:G101" si="2">F97/$F$103</f>
+        <v>0.2</v>
+      </c>
+      <c r="H97" t="str">
+        <f t="shared" si="1"/>
+        <v>Games &amp; 15 &amp; 20.00%\\</v>
+      </c>
+      <c r="I97" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E98" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="F98" s="40">
+        <f>11+2</f>
+        <v>13</v>
+      </c>
+      <c r="G98" s="39">
+        <f t="shared" si="2"/>
+        <v>0.17333333333333334</v>
+      </c>
+      <c r="H98" t="str">
+        <f t="shared" si="1"/>
+        <v>Autonomous driving &amp; 13 &amp; 17.33%\\</v>
+      </c>
+      <c r="I98" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="99" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E99" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F99" s="40">
+        <v>5</v>
+      </c>
+      <c r="G99" s="39">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H99" t="str">
+        <f t="shared" si="1"/>
+        <v>Control tasks &amp; 5 &amp; 6.67%\\</v>
+      </c>
+      <c r="I99" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="100" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E100" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F100" s="40">
+        <v>4</v>
+      </c>
+      <c r="G100" s="39">
+        <f t="shared" si="2"/>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="H100" t="str">
+        <f t="shared" si="1"/>
+        <v>Games &amp; 4 &amp; 5.33%\\</v>
+      </c>
+      <c r="I100" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="101" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E101" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F101" s="40">
+        <v>3</v>
+      </c>
+      <c r="G101" s="39">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="H101" t="str">
+        <f t="shared" si="1"/>
+        <v>Path Planning and Route planning &amp; 3 &amp; 4.00%\\</v>
+      </c>
+      <c r="I101" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F102" s="40"/>
+      <c r="G102" s="39"/>
+    </row>
+    <row r="103" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F103" s="40">
+        <f>SUM(F96:F101)</f>
+        <v>75</v>
+      </c>
+      <c r="G103" s="39"/>
+    </row>
+    <row r="104" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F104" s="40"/>
+      <c r="G104" s="39"/>
+    </row>
+    <row r="105" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F105" s="40"/>
+      <c r="G105" s="39"/>
+    </row>
+    <row r="106" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E106" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="F106" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="G106" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="H106" t="str">
+        <f t="shared" ref="H106:H116" si="3">_xlfn.CONCAT(E106," &amp; ",TEXT(F106,0)," &amp; ",TEXT(G106,".00%"), "\\")</f>
+        <v>IL Algorithm &amp; Articles &amp; %\\</v>
+      </c>
+      <c r="I106" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E107" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="F107" s="40">
+        <v>17</v>
+      </c>
+      <c r="G107" s="39">
+        <f>F107/$F$118</f>
+        <v>0.24285714285714285</v>
+      </c>
+      <c r="H107" t="str">
+        <f t="shared" si="3"/>
+        <v>Behavioral Cloning &amp; 17 &amp; 24.29%\\</v>
+      </c>
+      <c r="I107" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="108" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E108" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F108" s="40">
+        <v>9</v>
+      </c>
+      <c r="G108" s="39">
+        <f t="shared" ref="G108:G116" si="4">F108/$F$118</f>
+        <v>0.12857142857142856</v>
+      </c>
+      <c r="H108" t="str">
+        <f t="shared" si="3"/>
+        <v>Maximum Entropy IRL and Relative Entropy IRL &amp; 9 &amp; 12.86%\\</v>
+      </c>
+      <c r="I108" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="109" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E109" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F109" s="40">
+        <v>8</v>
+      </c>
+      <c r="G109" s="39">
+        <f t="shared" si="4"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="H109" t="str">
+        <f t="shared" si="3"/>
+        <v>IRL others (IRL from Observations, Cross-embodiment IRL) &amp; 8 &amp; 11.43%\\</v>
+      </c>
+      <c r="I109" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="110" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E110" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F110" s="40">
+        <v>7</v>
+      </c>
+      <c r="G110" s="39">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="H110" t="str">
+        <f t="shared" si="3"/>
+        <v>GAIL &amp; 7 &amp; 10.00%\\</v>
+      </c>
+      <c r="I110" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="111" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E111" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F111" s="40">
+        <v>6</v>
+      </c>
+      <c r="G111" s="39">
+        <f t="shared" si="4"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="H111" t="str">
+        <f t="shared" si="3"/>
+        <v>Imitation from Observation &amp; 6 &amp; 8.57%\\</v>
+      </c>
+      <c r="I111" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="112" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E112" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F112" s="40">
+        <v>5</v>
+      </c>
+      <c r="G112" s="39">
+        <f t="shared" si="4"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="H112" t="str">
+        <f t="shared" si="3"/>
+        <v>Bayesian IRL &amp; 5 &amp; 7.14%\\</v>
+      </c>
+      <c r="I112" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="113" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E113" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F113" s="40">
+        <v>4</v>
+      </c>
+      <c r="G113" s="39">
+        <f t="shared" si="4"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="H113" t="str">
+        <f t="shared" si="3"/>
+        <v>Adversarial IRL &amp; 4 &amp; 5.71%\\</v>
+      </c>
+      <c r="I113" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E114" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F114" s="40">
+        <v>4</v>
+      </c>
+      <c r="G114" s="39">
+        <f t="shared" si="4"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="H114" t="str">
+        <f t="shared" si="3"/>
+        <v>Maximum-margin IRL &amp; 4 &amp; 5.71%\\</v>
+      </c>
+      <c r="I114" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="115" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E115" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F115" s="40">
+        <v>3</v>
+      </c>
+      <c r="G115" s="39">
+        <f t="shared" si="4"/>
+        <v>4.2857142857142858E-2</v>
+      </c>
+      <c r="H115" t="str">
+        <f t="shared" si="3"/>
+        <v>Expert Support Estimation &amp; 3 &amp; 4.29%\\</v>
+      </c>
+      <c r="I115" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="116" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E116" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F116" s="40">
+        <v>7</v>
+      </c>
+      <c r="G116" s="39">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="H116" t="str">
+        <f t="shared" si="3"/>
+        <v>Others &amp; 7 &amp; 10.00%\\</v>
+      </c>
+      <c r="I116" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="118" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F118" s="5">
+        <f>SUM(F107:F116)</f>
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M71" xr:uid="{5103FA80-FD93-4C2C-B44E-DBC3C8F3DE31}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="BC from Observation"/>
-        <filter val="Conditional IL from Observations"/>
-        <filter val="Cross-domain II. from Observations"/>
-        <filter val="Generative Adversarial Imitation from Observation"/>
-        <filter val="Imitation from Observation"/>
-        <filter val="IRL from Observations"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L71" xr:uid="{5103FA80-FD93-4C2C-B44E-DBC3C8F3DE31}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E84:F90">
+    <sortCondition descending="1" ref="F84:F90"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F631AB-FFF0-4F7A-8CD6-E5FF36A61AAF}">
+  <dimension ref="A1:J71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="J8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="J10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>